<commit_message>
Updated new student of 5A
</commit_message>
<xml_diff>
--- a/2016-07-12/FIME-5A/Homework001/db/questions.xlsx
+++ b/2016-07-12/FIME-5A/Homework001/db/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>No</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Juan Gael Gonzalez Rodriguez</t>
+  </si>
+  <si>
+    <t>Luis Alejandro Urbina Gonzalez</t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB16"/>
+  <dimension ref="A1:BB17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:M16"/>
+      <selection activeCell="C17" sqref="C17:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,31 +1219,31 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:M16" ca="1" si="0">RANDBETWEEN(2,9)</f>
-        <v>9</v>
+        <f t="shared" ref="E2:M17" ca="1" si="0">RANDBETWEEN(2,9)</f>
+        <v>5</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
@@ -1248,15 +1251,15 @@
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
@@ -1268,47 +1271,47 @@
       </c>
       <c r="C3">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="C3:D16" ca="1" si="1">RANDBETWEEN(2,9)</f>
-        <v>2</v>
+        <f t="shared" ref="C3:D17" ca="1" si="1">RANDBETWEEN(2,9)</f>
+        <v>5</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="G3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J3">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="I3">
+      <c r="K3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L3">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="J3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
       <c r="M3">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
@@ -1320,47 +1323,47 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="K4">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
@@ -1372,47 +1375,47 @@
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="D5">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
@@ -1424,39 +1427,39 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
@@ -1464,7 +1467,7 @@
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
@@ -1476,43 +1479,43 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="E7">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="K7">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
@@ -1528,43 +1531,43 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="I8">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="0"/>
@@ -1580,7 +1583,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
@@ -1596,7 +1599,7 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
@@ -1604,23 +1607,23 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
@@ -1632,35 +1635,35 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
@@ -1668,11 +1671,11 @@
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
@@ -1684,47 +1687,47 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="J11">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="K11">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
@@ -1736,47 +1739,47 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H12">
+      <c r="L12">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="I12">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="K12">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L12">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
       <c r="M12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
@@ -1788,43 +1791,43 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="J13">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="0"/>
@@ -1840,7 +1843,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
@@ -1848,39 +1851,39 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="H14">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
@@ -1892,7 +1895,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
@@ -1900,7 +1903,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
@@ -1908,27 +1911,27 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="0"/>
@@ -1944,19 +1947,19 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
@@ -1964,11 +1967,11 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
@@ -1976,15 +1979,67 @@
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14155580</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new student to 5A
</commit_message>
<xml_diff>
--- a/2016-07-12/FIME-5A/Homework001/db/questions.xlsx
+++ b/2016-07-12/FIME-5A/Homework001/db/questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>No</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Luis Alejandro Urbina Gonzalez</t>
+  </si>
+  <si>
+    <t>Jose Waldo Quintana Aranda</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB17"/>
+  <dimension ref="A1:BB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:M17"/>
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,47 +1222,47 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:M18" ca="1" si="0">RANDBETWEEN(2,9)</f>
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:M17" ca="1" si="0">RANDBETWEEN(2,9)</f>
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="K2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
@@ -1271,47 +1274,47 @@
       </c>
       <c r="C3">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="C3:D17" ca="1" si="1">RANDBETWEEN(2,9)</f>
+        <f t="shared" ref="C3:D18" ca="1" si="1">RANDBETWEEN(2,9)</f>
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
@@ -1323,7 +1326,7 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
@@ -1335,23 +1338,23 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
@@ -1359,11 +1362,11 @@
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
@@ -1375,47 +1378,47 @@
       </c>
       <c r="C5">
         <f ca="1">RANDBETWEEN(2,9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="F5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
@@ -1427,47 +1430,47 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
@@ -1479,7 +1482,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
@@ -1487,7 +1490,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
@@ -1495,23 +1498,23 @@
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="0"/>
@@ -1519,7 +1522,7 @@
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
@@ -1539,19 +1542,19 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
@@ -1559,19 +1562,19 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
@@ -1583,7 +1586,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
@@ -1591,7 +1594,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
@@ -1599,31 +1602,31 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
@@ -1635,15 +1638,15 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
@@ -1651,31 +1654,31 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
@@ -1687,7 +1690,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
@@ -1695,39 +1698,39 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
@@ -1739,27 +1742,27 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
@@ -1767,19 +1770,19 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
@@ -1791,47 +1794,47 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
@@ -1843,23 +1846,23 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
@@ -1867,23 +1870,23 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
@@ -1895,23 +1898,23 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
@@ -1919,23 +1922,23 @@
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
@@ -1947,39 +1950,39 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="D16">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="I16">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="0"/>
@@ -1987,7 +1990,7 @@
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1999,47 +2002,99 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G17">
+      <c r="I17">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14629184</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E18">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="H17">
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H18">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="I17">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="K17">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="L17">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="M17">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+      <c r="I18">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>